<commit_message>
Finalise wet weather data and conductivity conversion
</commit_message>
<xml_diff>
--- a/matlab/Data_Import/WW_Conversion.xlsx
+++ b/matlab/Data_Import/WW_Conversion.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\Hawkesbury\matlab\Data_Import\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7C734E8F-B39C-4EAB-838D-43F70A644DF7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8C068D68-639D-4EB6-A223-458DD974D0FD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15990" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -113,9 +113,6 @@
     <t>Factor</t>
   </si>
   <si>
-    <t>Cond</t>
-  </si>
-  <si>
     <t>WQ_CAR_PH</t>
   </si>
   <si>
@@ -168,6 +165,9 @@
   </si>
   <si>
     <t>WQ_DIAG_OXY_SAT</t>
+  </si>
+  <si>
+    <t>COND</t>
   </si>
 </sst>
 </file>
@@ -583,8 +583,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:F32"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A5" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="B6" sqref="B6"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
@@ -615,7 +615,7 @@
         <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>44</v>
       </c>
       <c r="C3">
         <v>1</v>
@@ -629,7 +629,7 @@
         <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C4">
         <v>1</v>
@@ -643,7 +643,7 @@
         <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C5">
         <f>1000/32</f>
@@ -658,7 +658,7 @@
         <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C6">
         <v>1</v>
@@ -672,7 +672,7 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C7">
         <v>1</v>
@@ -686,7 +686,7 @@
         <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C8">
         <v>1</v>
@@ -700,7 +700,7 @@
         <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C9">
         <f>1000/31</f>
@@ -715,7 +715,7 @@
         <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C10">
         <f>1000/31</f>
@@ -730,7 +730,7 @@
         <v>9</v>
       </c>
       <c r="B11" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C11">
         <v>1</v>
@@ -744,7 +744,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C12">
         <v>1</v>
@@ -758,7 +758,7 @@
         <v>11</v>
       </c>
       <c r="B13" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C13">
         <f t="shared" ref="C13:C19" si="0">1000/14</f>
@@ -773,7 +773,7 @@
         <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C14">
         <f t="shared" si="0"/>
@@ -788,7 +788,7 @@
         <v>13</v>
       </c>
       <c r="B15" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="C15">
         <f t="shared" si="0"/>
@@ -803,7 +803,7 @@
         <v>14</v>
       </c>
       <c r="B16" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C16">
         <f t="shared" si="0"/>
@@ -818,7 +818,7 @@
         <v>15</v>
       </c>
       <c r="B17" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="C17">
         <f t="shared" si="0"/>
@@ -833,7 +833,7 @@
         <v>16</v>
       </c>
       <c r="B18" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C18">
         <f t="shared" si="0"/>
@@ -848,7 +848,7 @@
         <v>17</v>
       </c>
       <c r="B19" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C19">
         <f t="shared" si="0"/>
@@ -863,7 +863,7 @@
         <v>18</v>
       </c>
       <c r="B20" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C20">
         <v>1</v>
@@ -877,7 +877,7 @@
         <v>19</v>
       </c>
       <c r="B21" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C21">
         <v>1</v>
@@ -891,7 +891,7 @@
         <v>20</v>
       </c>
       <c r="B22" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C22">
         <f>1000/28.1</f>
@@ -906,7 +906,7 @@
         <v>21</v>
       </c>
       <c r="B23" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C23">
         <v>1</v>
@@ -920,7 +920,7 @@
         <v>22</v>
       </c>
       <c r="B24" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C24">
         <v>1</v>

</xml_diff>